<commit_message>
remove US values in bpmccs, update ptcf for hydro
</commit_message>
<xml_diff>
--- a/InputData/elec/PTCF/Peak Time Capacity Factors.xlsx
+++ b/InputData/elec/PTCF/Peak Time Capacity Factors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pembinainstitute.sharepoint.com/sites/PRO-EnergyPolicySimulator2021/Shared Documents/Research and Analysis/CANADA-inputData/elec/PTCF/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\Canada\canada-eps\InputData\elec\PTCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="437" documentId="8_{01D6FB42-3B39-4323-A21D-D79BA65E4289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{904083F7-C326-4835-82AC-18514BE2B0FE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A7786B-036C-45ED-ACD2-2B1F10BCF3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-4080" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14040" yWindow="2325" windowWidth="14010" windowHeight="12615" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="12" r:id="rId1"/>
@@ -995,87 +995,87 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.265625" customWidth="1"/>
-    <col min="2" max="2" width="50.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.59765625" customWidth="1"/>
-    <col min="8" max="8" width="53.73046875" customWidth="1"/>
+    <col min="1" max="1" width="9.26953125" customWidth="1"/>
+    <col min="2" max="2" width="50.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.6328125" customWidth="1"/>
+    <col min="8" max="8" width="53.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>7</v>
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>8</v>
       </c>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1102,44 +1102,44 @@
       <selection activeCell="B11" sqref="B11:M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.1328125" customWidth="1"/>
-    <col min="2" max="13" width="11.1328125" customWidth="1"/>
+    <col min="1" max="1" width="27.08984375" customWidth="1"/>
+    <col min="2" max="13" width="11.08984375" customWidth="1"/>
     <col min="14" max="14" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>20</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>44166</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>23</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>13137329</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>3448917</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>6834743</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>1321468</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>1459928</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>72273</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -2123,12 +2123,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -2136,12 +2136,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>5</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>6</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>7</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="356.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" ht="406" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>8</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>9</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>10</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>11</v>
       </c>
@@ -2229,12 +2229,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>3</v>
       </c>
@@ -2252,44 +2252,44 @@
       <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.86328125" customWidth="1"/>
-    <col min="2" max="13" width="11.86328125" customWidth="1"/>
-    <col min="14" max="14" width="12.1328125" customWidth="1"/>
+    <col min="1" max="1" width="45.81640625" customWidth="1"/>
+    <col min="2" max="13" width="11.81640625" customWidth="1"/>
+    <col min="14" max="14" width="12.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>20</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>44166</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>23</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>75454522</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>2434336</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>67670804</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -3068,7 +3068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>5285665</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>26344</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -3323,12 +3323,12 @@
         <v>37373</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -3336,12 +3336,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1</v>
       </c>
@@ -3349,7 +3349,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>3</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>4</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>5</v>
       </c>
@@ -3381,7 +3381,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>6</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>7</v>
       </c>
@@ -3397,7 +3397,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="342" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>8</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>9</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>10</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>11</v>
       </c>
@@ -3429,12 +3429,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>3</v>
       </c>
@@ -3452,44 +3452,44 @@
       <selection activeCell="B11" sqref="B11:M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.59765625" customWidth="1"/>
-    <col min="2" max="13" width="11.265625" customWidth="1"/>
-    <col min="14" max="14" width="10.59765625" customWidth="1"/>
+    <col min="1" max="1" width="28.6328125" customWidth="1"/>
+    <col min="2" max="13" width="11.26953125" customWidth="1"/>
+    <col min="14" max="14" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>20</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -3580,7 +3580,7 @@
         <v>44166</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>23</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -3672,7 +3672,7 @@
         <v>7644951</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -3756,7 +3756,7 @@
         <v>6776649</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -3840,7 +3840,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -3924,7 +3924,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -4092,7 +4092,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>521755</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -4344,7 +4344,7 @@
         <v>346491</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -4428,7 +4428,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -4512,12 +4512,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -4525,12 +4525,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2</v>
       </c>
@@ -4546,7 +4546,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>3</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>4</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>5</v>
       </c>
@@ -4570,7 +4570,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>6</v>
       </c>
@@ -4578,7 +4578,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>7</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="356.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" ht="391.5" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>8</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>9</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>10</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>11</v>
       </c>
@@ -4618,12 +4618,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>3</v>
       </c>
@@ -4641,44 +4641,44 @@
       <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.1328125" customWidth="1"/>
-    <col min="2" max="13" width="11.265625" customWidth="1"/>
-    <col min="14" max="14" width="11.19921875" customWidth="1"/>
+    <col min="1" max="1" width="35.08984375" customWidth="1"/>
+    <col min="2" max="13" width="11.26953125" customWidth="1"/>
+    <col min="14" max="14" width="11.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>20</v>
       </c>
@@ -4686,7 +4686,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -4763,7 +4763,7 @@
         <v>44550</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>23</v>
       </c>
@@ -4771,7 +4771,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -4852,7 +4852,7 @@
         <v>21081326</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>19813048</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -5014,7 +5014,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -5176,7 +5176,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -5257,7 +5257,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -5338,7 +5338,7 @@
         <v>183292</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -5419,7 +5419,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -5500,7 +5500,7 @@
         <v>1084941</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -5581,7 +5581,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -5662,12 +5662,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -5675,12 +5675,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1</v>
       </c>
@@ -5688,7 +5688,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2</v>
       </c>
@@ -5696,7 +5696,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>3</v>
       </c>
@@ -5704,7 +5704,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>4</v>
       </c>
@@ -5712,7 +5712,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>5</v>
       </c>
@@ -5720,7 +5720,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>6</v>
       </c>
@@ -5728,7 +5728,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>7</v>
       </c>
@@ -5736,7 +5736,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="356.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" ht="391.5" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>8</v>
       </c>
@@ -5744,7 +5744,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>9</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>10</v>
       </c>
@@ -5760,7 +5760,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>11</v>
       </c>
@@ -5768,12 +5768,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>3</v>
       </c>
@@ -5792,12 +5792,12 @@
       <selection pane="topRight" activeCell="Q54" sqref="Q54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
         <v>54</v>
       </c>
@@ -5819,7 +5819,7 @@
       <c r="Q1" s="9"/>
       <c r="R1" s="9"/>
     </row>
-    <row r="2" spans="1:18" ht="21" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:18" ht="21" x14ac:dyDescent="0.5">
       <c r="A2" s="10" t="s">
         <v>55</v>
       </c>
@@ -5841,7 +5841,7 @@
       <c r="Q2" s="9"/>
       <c r="R2" s="9"/>
     </row>
-    <row r="3" spans="1:18" ht="21" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:18" ht="21" x14ac:dyDescent="0.5">
       <c r="A3" s="10" t="s">
         <v>56</v>
       </c>
@@ -5863,7 +5863,7 @@
       <c r="Q3" s="9"/>
       <c r="R3" s="9"/>
     </row>
-    <row r="4" spans="1:18" ht="21" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:18" ht="21" x14ac:dyDescent="0.5">
       <c r="A4" s="10" t="s">
         <v>57</v>
       </c>
@@ -5885,7 +5885,7 @@
       <c r="Q4" s="9"/>
       <c r="R4" s="9"/>
     </row>
-    <row r="7" spans="1:18" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:18" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>58</v>
       </c>
@@ -5907,7 +5907,7 @@
       <c r="Q7" s="9"/>
       <c r="R7" s="9"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>59</v>
       </c>
@@ -5963,7 +5963,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>77</v>
       </c>
@@ -6019,7 +6019,7 @@
         <v>83287.27</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>78</v>
       </c>
@@ -6075,7 +6075,7 @@
         <v>14278.05</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>79</v>
       </c>
@@ -6131,7 +6131,7 @@
         <v>2337.0500000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>80</v>
       </c>
@@ -6187,7 +6187,7 @@
         <v>3202.15</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>81</v>
       </c>
@@ -6243,7 +6243,7 @@
         <v>12513</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
         <v>82</v>
       </c>
@@ -6299,7 +6299,7 @@
         <v>7976.8</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>83</v>
       </c>
@@ -6355,7 +6355,7 @@
         <v>26234.32</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>84</v>
       </c>
@@ -6411,7 +6411,7 @@
         <v>3134.53</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:18" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
         <v>53</v>
       </c>
@@ -6433,7 +6433,7 @@
       <c r="Q17" s="9"/>
       <c r="R17" s="9"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
         <v>59</v>
       </c>
@@ -6489,7 +6489,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>77</v>
       </c>
@@ -6545,7 +6545,7 @@
         <v>41111.35</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
         <v>78</v>
       </c>
@@ -6601,7 +6601,7 @@
         <v>4329.97</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>79</v>
       </c>
@@ -6657,7 +6657,7 @@
         <v>325.79000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>80</v>
       </c>
@@ -6713,7 +6713,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>81</v>
       </c>
@@ -6769,7 +6769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>82</v>
       </c>
@@ -6825,7 +6825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
         <v>83</v>
       </c>
@@ -6881,7 +6881,7 @@
         <v>649.13</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
         <v>84</v>
       </c>
@@ -6937,7 +6937,7 @@
         <v>311.04000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:18" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A28" s="11" t="s">
         <v>19</v>
       </c>
@@ -6959,7 +6959,7 @@
       <c r="Q28" s="9"/>
       <c r="R28" s="9"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
         <v>59</v>
       </c>
@@ -7015,7 +7015,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
         <v>77</v>
       </c>
@@ -7071,7 +7071,7 @@
         <v>9170.9</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
         <v>78</v>
       </c>
@@ -7127,7 +7127,7 @@
         <v>5536.45</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
         <v>79</v>
       </c>
@@ -7183,7 +7183,7 @@
         <v>465.4</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
         <v>80</v>
       </c>
@@ -7239,7 +7239,7 @@
         <v>2815.46</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
         <v>81</v>
       </c>
@@ -7295,7 +7295,7 @@
         <v>11808</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
         <v>82</v>
       </c>
@@ -7351,7 +7351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
         <v>83</v>
       </c>
@@ -7407,7 +7407,7 @@
         <v>10903.63</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
         <v>84</v>
       </c>
@@ -7463,7 +7463,7 @@
         <v>250.45</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:18" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A40" s="11" t="s">
         <v>51</v>
       </c>
@@ -7485,7 +7485,7 @@
       <c r="Q40" s="9"/>
       <c r="R40" s="9"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
         <v>59</v>
       </c>
@@ -7541,7 +7541,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
         <v>77</v>
       </c>
@@ -7597,7 +7597,7 @@
         <v>894.35</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
         <v>78</v>
       </c>
@@ -7653,7 +7653,7 @@
         <v>1745.76</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A44" s="9" t="s">
         <v>79</v>
       </c>
@@ -7709,7 +7709,7 @@
         <v>317.61</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
         <v>80</v>
       </c>
@@ -7765,7 +7765,7 @@
         <v>236.47</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
         <v>81</v>
       </c>
@@ -7821,7 +7821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
         <v>82</v>
       </c>
@@ -7877,7 +7877,7 @@
         <v>4993.8</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
         <v>83</v>
       </c>
@@ -7933,7 +7933,7 @@
         <v>10238.15</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="s">
         <v>84</v>
       </c>
@@ -7989,7 +7989,7 @@
         <v>7.15</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:18" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A51" s="11" t="s">
         <v>52</v>
       </c>
@@ -8011,7 +8011,7 @@
       <c r="Q51" s="9"/>
       <c r="R51" s="9"/>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="s">
         <v>59</v>
       </c>
@@ -8067,7 +8067,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
         <v>77</v>
       </c>
@@ -8123,7 +8123,7 @@
         <v>16017.47</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A54" s="9" t="s">
         <v>78</v>
       </c>
@@ -8179,7 +8179,7 @@
         <v>732.25</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A55" s="9" t="s">
         <v>79</v>
       </c>
@@ -8235,7 +8235,7 @@
         <v>927.79</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A56" s="9" t="s">
         <v>80</v>
       </c>
@@ -8291,7 +8291,7 @@
         <v>23.28</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
         <v>81</v>
       </c>
@@ -8347,7 +8347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A58" s="9" t="s">
         <v>82</v>
       </c>
@@ -8403,7 +8403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
         <v>83</v>
       </c>
@@ -8459,7 +8459,7 @@
         <v>520.33000000000004</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A60" s="9" t="s">
         <v>84</v>
       </c>
@@ -8515,8 +8515,8 @@
         <v>122.46</v>
       </c>
     </row>
-    <row r="61" spans="1:18" ht="18.95" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="62" spans="1:18" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="62" spans="1:18" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A62" s="11"/>
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
@@ -8536,7 +8536,7 @@
       <c r="Q62" s="9"/>
       <c r="R62" s="9"/>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A63" s="9"/>
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
@@ -8556,7 +8556,7 @@
       <c r="Q63" s="9"/>
       <c r="R63" s="9"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A64" s="9"/>
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
@@ -8576,7 +8576,7 @@
       <c r="Q64" s="9"/>
       <c r="R64" s="9"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A65" s="9"/>
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
@@ -8596,7 +8596,7 @@
       <c r="Q65" s="9"/>
       <c r="R65" s="9"/>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A66" s="9"/>
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
@@ -8616,7 +8616,7 @@
       <c r="Q66" s="9"/>
       <c r="R66" s="9"/>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A67" s="9"/>
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
@@ -8636,7 +8636,7 @@
       <c r="Q67" s="9"/>
       <c r="R67" s="9"/>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A68" s="9"/>
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
@@ -8656,7 +8656,7 @@
       <c r="Q68" s="9"/>
       <c r="R68" s="9"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A69" s="9"/>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
@@ -8676,7 +8676,7 @@
       <c r="Q69" s="9"/>
       <c r="R69" s="9"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A70" s="9"/>
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
@@ -8696,7 +8696,7 @@
       <c r="Q70" s="9"/>
       <c r="R70" s="9"/>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A71" s="9"/>
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
@@ -8716,7 +8716,7 @@
       <c r="Q71" s="9"/>
       <c r="R71" s="9"/>
     </row>
-    <row r="73" spans="1:18" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:18" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A73" s="11"/>
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
@@ -8736,7 +8736,7 @@
       <c r="Q73" s="9"/>
       <c r="R73" s="9"/>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A74" s="9"/>
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
@@ -8756,7 +8756,7 @@
       <c r="Q74" s="9"/>
       <c r="R74" s="9"/>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A75" s="9"/>
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
@@ -8776,7 +8776,7 @@
       <c r="Q75" s="9"/>
       <c r="R75" s="9"/>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A76" s="9"/>
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
@@ -8796,7 +8796,7 @@
       <c r="Q76" s="9"/>
       <c r="R76" s="9"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A77" s="9"/>
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
@@ -8816,7 +8816,7 @@
       <c r="Q77" s="9"/>
       <c r="R77" s="9"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A78" s="9"/>
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
@@ -8836,7 +8836,7 @@
       <c r="Q78" s="9"/>
       <c r="R78" s="9"/>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A79" s="9"/>
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
@@ -8856,7 +8856,7 @@
       <c r="Q79" s="9"/>
       <c r="R79" s="9"/>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A80" s="9"/>
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
@@ -8876,7 +8876,7 @@
       <c r="Q80" s="9"/>
       <c r="R80" s="9"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A81" s="9"/>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
@@ -8896,7 +8896,7 @@
       <c r="Q81" s="9"/>
       <c r="R81" s="9"/>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A82" s="9"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
@@ -8916,7 +8916,7 @@
       <c r="Q82" s="9"/>
       <c r="R82" s="9"/>
     </row>
-    <row r="84" spans="1:18" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:18" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A84" s="11"/>
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
@@ -8936,7 +8936,7 @@
       <c r="Q84" s="9"/>
       <c r="R84" s="9"/>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A85" s="9"/>
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
@@ -8956,7 +8956,7 @@
       <c r="Q85" s="9"/>
       <c r="R85" s="9"/>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A86" s="9"/>
       <c r="B86" s="9"/>
       <c r="C86" s="9"/>
@@ -8976,7 +8976,7 @@
       <c r="Q86" s="9"/>
       <c r="R86" s="9"/>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A87" s="9"/>
       <c r="B87" s="9"/>
       <c r="C87" s="9"/>
@@ -8996,7 +8996,7 @@
       <c r="Q87" s="9"/>
       <c r="R87" s="9"/>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A88" s="9"/>
       <c r="B88" s="9"/>
       <c r="C88" s="9"/>
@@ -9016,7 +9016,7 @@
       <c r="Q88" s="9"/>
       <c r="R88" s="9"/>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A89" s="9"/>
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
@@ -9036,7 +9036,7 @@
       <c r="Q89" s="9"/>
       <c r="R89" s="9"/>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A90" s="9"/>
       <c r="B90" s="9"/>
       <c r="C90" s="9"/>
@@ -9056,7 +9056,7 @@
       <c r="Q90" s="9"/>
       <c r="R90" s="9"/>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A91" s="9"/>
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
@@ -9076,7 +9076,7 @@
       <c r="Q91" s="9"/>
       <c r="R91" s="9"/>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A92" s="9"/>
       <c r="B92" s="9"/>
       <c r="C92" s="9"/>
@@ -9096,7 +9096,7 @@
       <c r="Q92" s="9"/>
       <c r="R92" s="9"/>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A93" s="9"/>
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
@@ -9116,7 +9116,7 @@
       <c r="Q93" s="9"/>
       <c r="R93" s="9"/>
     </row>
-    <row r="95" spans="1:18" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:18" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A95" s="11"/>
       <c r="B95" s="9"/>
       <c r="C95" s="9"/>
@@ -9136,7 +9136,7 @@
       <c r="Q95" s="9"/>
       <c r="R95" s="9"/>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A96" s="9"/>
       <c r="B96" s="9"/>
       <c r="C96" s="9"/>
@@ -9156,7 +9156,7 @@
       <c r="Q96" s="9"/>
       <c r="R96" s="9"/>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A97" s="9"/>
       <c r="B97" s="9"/>
       <c r="C97" s="9"/>
@@ -9176,7 +9176,7 @@
       <c r="Q97" s="9"/>
       <c r="R97" s="9"/>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A98" s="9"/>
       <c r="B98" s="9"/>
       <c r="C98" s="9"/>
@@ -9196,7 +9196,7 @@
       <c r="Q98" s="9"/>
       <c r="R98" s="9"/>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A99" s="9"/>
       <c r="B99" s="9"/>
       <c r="C99" s="9"/>
@@ -9216,7 +9216,7 @@
       <c r="Q99" s="9"/>
       <c r="R99" s="9"/>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A100" s="9"/>
       <c r="B100" s="9"/>
       <c r="C100" s="9"/>
@@ -9236,7 +9236,7 @@
       <c r="Q100" s="9"/>
       <c r="R100" s="9"/>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A101" s="9"/>
       <c r="B101" s="9"/>
       <c r="C101" s="9"/>
@@ -9256,7 +9256,7 @@
       <c r="Q101" s="9"/>
       <c r="R101" s="9"/>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A102" s="9"/>
       <c r="B102" s="9"/>
       <c r="C102" s="9"/>
@@ -9276,7 +9276,7 @@
       <c r="Q102" s="9"/>
       <c r="R102" s="9"/>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A103" s="9"/>
       <c r="B103" s="9"/>
       <c r="C103" s="9"/>
@@ -9296,7 +9296,7 @@
       <c r="Q103" s="9"/>
       <c r="R103" s="9"/>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A104" s="9"/>
       <c r="B104" s="9"/>
       <c r="C104" s="9"/>
@@ -9325,20 +9325,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.73046875" customWidth="1"/>
-    <col min="3" max="3" width="9.3984375" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7265625" customWidth="1"/>
+    <col min="3" max="3" width="9.36328125" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>85</v>
       </c>
@@ -9346,7 +9346,7 @@
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>86</v>
       </c>
@@ -9357,7 +9357,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>51</v>
       </c>
@@ -9368,7 +9368,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>19</v>
       </c>
@@ -9379,7 +9379,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>91</v>
       </c>
@@ -9390,7 +9390,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>53</v>
       </c>
@@ -9401,7 +9401,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>92</v>
       </c>
@@ -9409,7 +9409,7 @@
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>86</v>
       </c>
@@ -9426,7 +9426,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -9446,7 +9446,7 @@
         <v>72958398</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -9466,7 +9466,7 @@
         <v>72958398</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -9486,7 +9486,7 @@
         <v>1997591</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -9506,7 +9506,7 @@
         <v>4119223</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -9526,7 +9526,7 @@
         <v>25547</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -9546,7 +9546,7 @@
         <v>13353087</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -9566,7 +9566,7 @@
         <v>90155270</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -9586,7 +9586,7 @@
         <v>37687913</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -9606,7 +9606,7 @@
         <v>11253753</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -9626,7 +9626,7 @@
         <v>2176592</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>91</v>
       </c>
@@ -9646,7 +9646,7 @@
         <v>5599378</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>91</v>
       </c>
@@ -9666,7 +9666,7 @@
         <v>60434039</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>91</v>
       </c>
@@ -9686,7 +9686,7 @@
         <v>1422361</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>91</v>
       </c>
@@ -9706,7 +9706,7 @@
         <v>1558</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -9726,7 +9726,7 @@
         <v>2212202</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -9746,7 +9746,7 @@
         <v>201007493</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -9766,7 +9766,7 @@
         <v>10641247</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -9799,19 +9799,19 @@
   </sheetPr>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.265625" customWidth="1"/>
+    <col min="1" max="1" width="24.26953125" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="12.86328125" customWidth="1"/>
-    <col min="6" max="6" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>101</v>
       </c>
@@ -9822,7 +9822,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>95</v>
       </c>
@@ -9833,7 +9833,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>96</v>
       </c>
@@ -9844,7 +9844,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -9855,20 +9855,18 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>97</v>
       </c>
       <c r="B5" s="4">
-        <f t="array" ref="B5">IFERROR(SUMPRODUCT(IF(Calculations!$B$13:$B$31=PTCF!A5,Calculations!$C$13:$C$31),IF(Calculations!$B$13:$B$31=PTCF!A5,Calculations!$E$13:$E$31))/SUMIFS(Calculations!$E$13:$E$31,Calculations!$B$13:$B$31,PTCF!A5,Calculations!$C$13:$C$31,"&lt;&gt;"&amp;""),1)</f>
-        <v>0.47867023811791642</v>
+        <v>1</v>
       </c>
       <c r="C5" s="4">
-        <f t="array" ref="C5">IFERROR(SUMPRODUCT(IF(Calculations!$B$13:$B$31=PTCF!A5,Calculations!$D$13:$D$31),IF(Calculations!$B$13:$B$31=PTCF!A5,Calculations!$E$13:$E$31))/SUMIFS(Calculations!$E$13:$E$31,Calculations!$B$13:$B$31,PTCF!A5,Calculations!$D$13:$D$31,"&lt;&gt;"&amp;""),1)</f>
-        <v>0.59805965841864694</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>98</v>
       </c>
@@ -9881,7 +9879,7 @@
         <v>0.34825721327847176</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>99</v>
       </c>
@@ -9894,7 +9892,7 @@
         <v>3.0450909453317451E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -9907,7 +9905,7 @@
         <v>3.0450909453317451E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>105</v>
       </c>
@@ -9920,7 +9918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>106</v>
       </c>
@@ -9933,7 +9931,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>107</v>
       </c>
@@ -9944,7 +9942,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>96</v>
       </c>
@@ -9955,7 +9953,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>108</v>
       </c>
@@ -9968,7 +9966,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>109</v>
       </c>
@@ -9981,7 +9979,7 @@
         <v>0.34825721327847176</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>110</v>
       </c>
@@ -9992,7 +9990,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>111</v>
       </c>
@@ -10003,7 +10001,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>112</v>
       </c>
@@ -10022,6 +10020,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <of2ed5e60f3c4f8984f283882cb94320 xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
@@ -10039,15 +10046,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10311,6 +10309,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFAA4812-A3AB-4DC7-96BF-ABB79AD356F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95045A36-27E4-4EF7-BE1B-41B196E8F570}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -10328,14 +10334,22 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFAA4812-A3AB-4DC7-96BF-ABB79AD356F2}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F601648-D229-44DF-B80E-8AA867842C20}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="52604411-7aeb-406e-8b34-4ce79a7293cc"/>
+    <ds:schemaRef ds:uri="de340059-046a-4f1a-8b62-ade039df3700"/>
+    <ds:schemaRef ds:uri="d580559a-617d-4d7d-8fb9-71ff64b58360"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F601648-D229-44DF-B80E-8AA867842C20}"/>
 </file>
</xml_diff>